<commit_message>
Updated PCB design files
</commit_message>
<xml_diff>
--- a/H_bridge_PCB_Design/BOM/H_bridge_PCB.xlsx
+++ b/H_bridge_PCB_Design/BOM/H_bridge_PCB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\Studiumsstoff\Master\Forschungspraxis\H_bridge_PCB\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\Studiumsstoff\Master\Forschungspraxis\git\H_bridge_PCB_Design\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BBFC1DF9-A7E8-4427-8ED3-9817EC7BDBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFAB3BC2-E3F1-479D-AFFB-EC5638C073AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{328AC39E-EA40-4E6B-9B7B-7CFEE2F9DA27}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4801B267-E72B-4B2D-89FC-8797BE10652E}"/>
   </bookViews>
   <sheets>
     <sheet name="H_bridge_PCB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="144">
   <si>
     <t>Value</t>
   </si>
@@ -37,28 +37,28 @@
     <t>LCSC Part#</t>
   </si>
   <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>MKP1847H55025JK2</t>
-  </si>
-  <si>
-    <t>SamacSys_Parts:MKP1847H55025JK2</t>
+    <t>C13,C16,C22</t>
+  </si>
+  <si>
+    <t>MKS4C042204C00KSSD</t>
+  </si>
+  <si>
+    <t>SamacSys_Parts:MKS4C042204C00KSSD</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>ACS37800KMACTR-030B3-I2C</t>
+  </si>
+  <si>
+    <t>ACS37002LMCA050U5</t>
   </si>
   <si>
     <t>Nicht bestÃ¼cken</t>
   </si>
   <si>
-    <t>IC5</t>
-  </si>
-  <si>
-    <t>ACS37800KMACTR-030B3-I2C</t>
-  </si>
-  <si>
-    <t>ACS37002LMCA050U5</t>
-  </si>
-  <si>
-    <t>J1,J2,J3,J4,J5</t>
+    <t>J1,J2,J3,J4,J5,J6,J7,J8,J9,J10,J11</t>
   </si>
   <si>
     <t>TMS-102-21-G-S</t>
@@ -1312,12 +1312,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FAF6A6-D1B2-4FA1-87E0-14DEEE89FF3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6966F2-FE62-4D83-B833-2BD309AF3DDC}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1352,27 +1350,24 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1386,10 +1381,10 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1406,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1423,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1440,7 +1435,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1457,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1474,7 +1469,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1491,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>